<commit_message>
column to collumn ha
</commit_message>
<xml_diff>
--- a/Example Data/Labware Excel Input.xlsx
+++ b/Example Data/Labware Excel Input.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daviahsmith/Downloads/Labware-Definer/Example Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED5217A-5661-BF41-81DD-079421259D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="wKvA2Y0N+qJv8fAkGha3TGvyRIxApfrAJ5pjGarnPtM="/>
@@ -16,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="106">
   <si>
     <t>A hash in this column will prevent the row being read in</t>
   </si>
@@ -328,29 +337,38 @@
   </si>
   <si>
     <t>3851</t>
+  </si>
+  <si>
+    <t>96-well V-bottom Nunc clear</t>
+  </si>
+  <si>
+    <t>REAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -358,41 +376,44 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -582,50 +603,50 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3.0" ySplit="2.0" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="D1" sqref="D1" pane="topRight"/>
-      <selection activeCell="A3" sqref="A3" pane="bottomLeft"/>
-      <selection activeCell="D3" sqref="D3" pane="bottomRight"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="4.29"/>
-    <col customWidth="1" min="2" max="2" width="25.43"/>
-    <col customWidth="1" min="3" max="3" width="14.14"/>
-    <col customWidth="1" min="4" max="4" width="15.29"/>
-    <col customWidth="1" min="5" max="5" width="10.29"/>
-    <col customWidth="1" min="6" max="6" width="13.43"/>
-    <col customWidth="1" min="7" max="7" width="15.57"/>
-    <col customWidth="1" min="8" max="8" width="16.0"/>
-    <col customWidth="1" min="9" max="9" width="17.14"/>
-    <col customWidth="1" min="10" max="10" width="11.43"/>
-    <col customWidth="1" min="11" max="11" width="18.14"/>
-    <col customWidth="1" min="12" max="12" width="11.14"/>
-    <col customWidth="1" min="13" max="13" width="18.14"/>
-    <col customWidth="1" min="14" max="14" width="23.0"/>
-    <col customWidth="1" min="15" max="15" width="15.14"/>
-    <col customWidth="1" min="16" max="16" width="14.86"/>
-    <col customWidth="1" min="17" max="17" width="18.86"/>
-    <col customWidth="1" min="18" max="18" width="21.29"/>
-    <col customWidth="1" min="19" max="22" width="14.43"/>
-    <col customWidth="1" min="23" max="23" width="12.14"/>
-    <col customWidth="1" min="24" max="24" width="14.86"/>
-    <col customWidth="1" min="25" max="25" width="13.57"/>
-    <col customWidth="1" min="26" max="26" width="8.71"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.5" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="15.5" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" customWidth="1"/>
+    <col min="10" max="10" width="11.5" customWidth="1"/>
+    <col min="11" max="11" width="18.1640625" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" customWidth="1"/>
+    <col min="13" max="13" width="18.1640625" customWidth="1"/>
+    <col min="14" max="14" width="23" customWidth="1"/>
+    <col min="15" max="15" width="15.1640625" customWidth="1"/>
+    <col min="16" max="16" width="14.83203125" customWidth="1"/>
+    <col min="17" max="17" width="18.83203125" customWidth="1"/>
+    <col min="18" max="18" width="21.33203125" customWidth="1"/>
+    <col min="19" max="22" width="14.5" customWidth="1"/>
+    <col min="23" max="23" width="12.1640625" customWidth="1"/>
+    <col min="24" max="24" width="14.83203125" customWidth="1"/>
+    <col min="25" max="25" width="13.5" customWidth="1"/>
+    <col min="26" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -680,10 +701,10 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="U1" s="1" t="s">
@@ -702,88 +723,88 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Y2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z2" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -793,10 +814,10 @@
         <v>53</v>
       </c>
       <c r="E3" s="1">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="F3" s="1">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="G3" s="1">
         <v>128.32</v>
@@ -808,10 +829,10 @@
         <v>15.61</v>
       </c>
       <c r="J3" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="K3" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>54</v>
@@ -841,10 +862,10 @@
         <v>6.41</v>
       </c>
       <c r="U3" s="1">
-        <v>112.0</v>
+        <v>112</v>
       </c>
       <c r="V3" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>56</v>
@@ -859,8 +880,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -870,10 +891,10 @@
         <v>60</v>
       </c>
       <c r="E4" s="1">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="F4" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G4" s="1">
         <v>128.15</v>
@@ -885,7 +906,7 @@
         <v>14.93</v>
       </c>
       <c r="J4" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="K4" s="1">
         <v>11.4</v>
@@ -900,7 +921,7 @@
         <v>7.8</v>
       </c>
       <c r="O4" s="1">
-        <v>4.56</v>
+        <v>4.5599999999999996</v>
       </c>
       <c r="P4" s="1">
         <v>5.93</v>
@@ -918,10 +939,10 @@
         <v>7.46</v>
       </c>
       <c r="U4" s="1">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="V4" s="1">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>62</v>
@@ -936,8 +957,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
         <v>63</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -947,13 +968,13 @@
         <v>65</v>
       </c>
       <c r="E5" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="F5" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="G5" s="1">
-        <v>128.02</v>
+        <v>128.02000000000001</v>
       </c>
       <c r="H5" s="1">
         <v>86.54</v>
@@ -962,7 +983,7 @@
         <v>14.55</v>
       </c>
       <c r="J5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="K5" s="1">
         <v>10.1</v>
@@ -995,10 +1016,10 @@
         <v>6.1</v>
       </c>
       <c r="U5" s="1">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="V5" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="W5" s="1" t="s">
         <v>67</v>
@@ -1013,8 +1034,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1024,10 +1045,10 @@
         <v>69</v>
       </c>
       <c r="E6" s="1">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="F6" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G6" s="1">
         <v>127.16</v>
@@ -1039,7 +1060,7 @@
         <v>15.48</v>
       </c>
       <c r="J6" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="K6" s="1">
         <v>10.6</v>
@@ -1057,13 +1078,13 @@
         <v>4.2</v>
       </c>
       <c r="P6" s="1">
-        <v>4.61</v>
+        <v>4.6100000000000003</v>
       </c>
       <c r="Q6" s="1">
         <v>13.13</v>
       </c>
       <c r="R6" s="1">
-        <v>10.22</v>
+        <v>10.220000000000001</v>
       </c>
       <c r="S6" s="1">
         <v>6.38</v>
@@ -1072,10 +1093,10 @@
         <v>6.33</v>
       </c>
       <c r="U6" s="1">
-        <v>112.0</v>
+        <v>112</v>
       </c>
       <c r="V6" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="W6" s="1" t="s">
         <v>62</v>
@@ -1090,8 +1111,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="B7" s="2" t="s">
+    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1101,10 +1122,10 @@
         <v>71</v>
       </c>
       <c r="E7" s="1">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="F7" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G7" s="1">
         <v>128.97</v>
@@ -1116,7 +1137,7 @@
         <v>15.4</v>
       </c>
       <c r="J7" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="K7" s="1">
         <v>11.9</v>
@@ -1149,10 +1170,10 @@
         <v>7.33</v>
       </c>
       <c r="U7" s="1">
-        <v>360.0</v>
+        <v>360</v>
       </c>
       <c r="V7" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="W7" s="1" t="s">
         <v>62</v>
@@ -1167,8 +1188,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
-      <c r="B8" s="2" t="s">
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1178,10 +1199,10 @@
         <v>74</v>
       </c>
       <c r="E8" s="1">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="F8" s="1">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="G8" s="1">
         <v>128.5</v>
@@ -1193,7 +1214,7 @@
         <v>15.39</v>
       </c>
       <c r="J8" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K8" s="1">
         <v>11.8</v>
@@ -1226,10 +1247,10 @@
         <v>7.56</v>
       </c>
       <c r="U8" s="1">
-        <v>112.0</v>
+        <v>112</v>
       </c>
       <c r="V8" s="1">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="W8" s="1" t="s">
         <v>62</v>
@@ -1244,8 +1265,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="B9" s="2" t="s">
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1255,10 +1276,10 @@
         <v>76</v>
       </c>
       <c r="E9" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="F9" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="G9" s="1">
         <v>128.06</v>
@@ -1270,7 +1291,7 @@
         <v>13.01</v>
       </c>
       <c r="J9" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="K9" s="1">
         <v>11.8</v>
@@ -1303,10 +1324,10 @@
         <v>9.81</v>
       </c>
       <c r="U9" s="1">
-        <v>360.0</v>
+        <v>360</v>
       </c>
       <c r="V9" s="1">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="W9" s="1" t="s">
         <v>62</v>
@@ -1321,8 +1342,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" ht="14.25" customHeight="1">
-      <c r="B10" s="2" t="s">
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1332,10 +1353,10 @@
         <v>78</v>
       </c>
       <c r="E10" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="F10" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="G10" s="1">
         <v>127.13</v>
@@ -1347,7 +1368,7 @@
         <v>15.03</v>
       </c>
       <c r="J10" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="1">
         <v>11.4</v>
@@ -1377,13 +1398,13 @@
         <v>9.23</v>
       </c>
       <c r="T10" s="1">
-        <v>9.2</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="U10" s="1">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="V10" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="W10" s="1" t="s">
         <v>62</v>
@@ -1398,8 +1419,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="B11" s="2" t="s">
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1409,10 +1430,10 @@
         <v>81</v>
       </c>
       <c r="E11" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="F11" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G11" s="1">
         <v>128.22</v>
@@ -1424,7 +1445,7 @@
         <v>13.63</v>
       </c>
       <c r="J11" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="K11" s="1">
         <v>10.1</v>
@@ -1457,10 +1478,10 @@
         <v>6.29</v>
       </c>
       <c r="U11" s="1">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="V11" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="W11" s="1" t="s">
         <v>67</v>
@@ -1475,11 +1496,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>82</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1489,10 +1510,10 @@
         <v>83</v>
       </c>
       <c r="E12" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="F12" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G12" s="1">
         <v>127.01</v>
@@ -1504,7 +1525,7 @@
         <v>13.63</v>
       </c>
       <c r="J12" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="K12" s="1">
         <v>11.9</v>
@@ -1534,13 +1555,13 @@
         <v>6.27</v>
       </c>
       <c r="T12" s="1">
-        <v>9.13</v>
+        <v>9.1300000000000008</v>
       </c>
       <c r="U12" s="1">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="V12" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="W12" s="1" t="s">
         <v>56</v>
@@ -1555,11 +1576,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
+    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>84</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1569,10 +1590,10 @@
         <v>85</v>
       </c>
       <c r="E13" s="1">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="F13" s="1">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="G13" s="1">
         <v>127.2</v>
@@ -1584,7 +1605,7 @@
         <v>15.34</v>
       </c>
       <c r="J13" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K13" s="1">
         <v>10.4</v>
@@ -1617,10 +1638,10 @@
         <v>6.9</v>
       </c>
       <c r="U13" s="1">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="V13" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="W13" s="1" t="s">
         <v>56</v>
@@ -1635,8 +1656,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" ht="14.25" customHeight="1">
-      <c r="B14" s="2" t="s">
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1646,13 +1667,13 @@
         <v>87</v>
       </c>
       <c r="E14" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="F14" s="1">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="G14" s="1">
-        <v>128.23</v>
+        <v>128.22999999999999</v>
       </c>
       <c r="H14" s="1">
         <v>85.37</v>
@@ -1661,10 +1682,10 @@
         <v>14.44</v>
       </c>
       <c r="J14" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K14" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>54</v>
@@ -1691,13 +1712,13 @@
         <v>8.27</v>
       </c>
       <c r="T14" s="1">
-        <v>8.2</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="U14" s="1">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="V14" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="W14" s="1" t="s">
         <v>62</v>
@@ -1712,8 +1733,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
-      <c r="B15" s="2" t="s">
+    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1723,10 +1744,10 @@
         <v>89</v>
       </c>
       <c r="E15" s="1">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="F15" s="1">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="G15" s="1">
         <v>127.76</v>
@@ -1738,7 +1759,7 @@
         <v>13.11</v>
       </c>
       <c r="J15" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="K15" s="1">
         <v>11.6</v>
@@ -1771,10 +1792,10 @@
         <v>5.48</v>
       </c>
       <c r="U15" s="1">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="V15" s="1">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="W15" s="1" t="s">
         <v>56</v>
@@ -1789,8 +1810,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
-      <c r="B16" s="2" t="s">
+    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1800,10 +1821,10 @@
         <v>91</v>
       </c>
       <c r="E16" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="F16" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G16" s="1">
         <v>128.53</v>
@@ -1815,7 +1836,7 @@
         <v>15.88</v>
       </c>
       <c r="J16" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="K16" s="1">
         <v>10.7</v>
@@ -1827,7 +1848,7 @@
         <v>79</v>
       </c>
       <c r="N16" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="O16" s="1">
         <v>6.58</v>
@@ -1848,10 +1869,10 @@
         <v>6.27</v>
       </c>
       <c r="U16" s="1">
-        <v>360.0</v>
+        <v>360</v>
       </c>
       <c r="V16" s="1">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="W16" s="1" t="s">
         <v>62</v>
@@ -1866,8 +1887,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
-      <c r="B17" s="2" t="s">
+    <row r="17" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -1877,10 +1898,10 @@
         <v>93</v>
       </c>
       <c r="E17" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="F17" s="1">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="G17" s="1">
         <v>128.44</v>
@@ -1892,7 +1913,7 @@
         <v>13.21</v>
       </c>
       <c r="J17" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="K17" s="1">
         <v>11.7</v>
@@ -1904,7 +1925,7 @@
         <v>61</v>
       </c>
       <c r="N17" s="1">
-        <v>8.7</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="O17" s="1">
         <v>5.12</v>
@@ -1925,10 +1946,10 @@
         <v>9.17</v>
       </c>
       <c r="U17" s="1">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="V17" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="W17" s="1" t="s">
         <v>56</v>
@@ -1943,8 +1964,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" ht="14.25" customHeight="1">
-      <c r="B18" s="2" t="s">
+    <row r="18" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
         <v>94</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1954,10 +1975,10 @@
         <v>95</v>
       </c>
       <c r="E18" s="1">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="F18" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="G18" s="1">
         <v>127.62</v>
@@ -1969,7 +1990,7 @@
         <v>13.03</v>
       </c>
       <c r="J18" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="K18" s="1">
         <v>10.3</v>
@@ -1981,7 +2002,7 @@
         <v>55</v>
       </c>
       <c r="N18" s="1">
-        <v>8.7</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="O18" s="1">
         <v>5.14</v>
@@ -2002,10 +2023,10 @@
         <v>8.19</v>
       </c>
       <c r="U18" s="1">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="V18" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="W18" s="1" t="s">
         <v>67</v>
@@ -2020,8 +2041,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" ht="14.25" customHeight="1">
-      <c r="B19" s="2" t="s">
+    <row r="19" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -2031,10 +2052,10 @@
         <v>97</v>
       </c>
       <c r="E19" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="F19" s="1">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="G19" s="1">
         <v>127.76</v>
@@ -2043,10 +2064,10 @@
         <v>85.27</v>
       </c>
       <c r="I19" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="J19" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="K19" s="1">
         <v>11.1</v>
@@ -2064,7 +2085,7 @@
         <v>6.48</v>
       </c>
       <c r="P19" s="1">
-        <v>4.52</v>
+        <v>4.5199999999999996</v>
       </c>
       <c r="Q19" s="1">
         <v>14.01</v>
@@ -2073,16 +2094,16 @@
         <v>11.95</v>
       </c>
       <c r="S19" s="1">
-        <v>8.62</v>
+        <v>8.6199999999999992</v>
       </c>
       <c r="T19" s="1">
         <v>8.92</v>
       </c>
       <c r="U19" s="1">
-        <v>360.0</v>
+        <v>360</v>
       </c>
       <c r="V19" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="W19" s="1" t="s">
         <v>62</v>
@@ -2097,8 +2118,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" ht="14.25" customHeight="1">
-      <c r="B20" s="2" t="s">
+    <row r="20" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -2108,10 +2129,10 @@
         <v>99</v>
       </c>
       <c r="E20" s="1">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="F20" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="G20" s="1">
         <v>127.74</v>
@@ -2123,7 +2144,7 @@
         <v>13.19</v>
       </c>
       <c r="J20" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="1">
         <v>11.3</v>
@@ -2156,10 +2177,10 @@
         <v>5.6</v>
       </c>
       <c r="U20" s="1">
-        <v>360.0</v>
+        <v>360</v>
       </c>
       <c r="V20" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="W20" s="1" t="s">
         <v>62</v>
@@ -2174,8 +2195,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" ht="14.25" customHeight="1">
-      <c r="B21" s="2" t="s">
+    <row r="21" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
         <v>100</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -2185,10 +2206,10 @@
         <v>101</v>
       </c>
       <c r="E21" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="F21" s="1">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="G21" s="1">
         <v>128.53</v>
@@ -2200,7 +2221,7 @@
         <v>15.47</v>
       </c>
       <c r="J21" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="K21" s="1">
         <v>11.2</v>
@@ -2227,16 +2248,16 @@
         <v>9.43</v>
       </c>
       <c r="S21" s="1">
-        <v>9.28</v>
+        <v>9.2799999999999994</v>
       </c>
       <c r="T21" s="1">
         <v>6.65</v>
       </c>
       <c r="U21" s="1">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="V21" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="W21" s="1" t="s">
         <v>67</v>
@@ -2251,8 +2272,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" ht="14.25" customHeight="1">
-      <c r="B22" s="2" t="s">
+    <row r="22" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -2262,10 +2283,10 @@
         <v>103</v>
       </c>
       <c r="E22" s="1">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="F22" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="G22" s="1">
         <v>127.4</v>
@@ -2277,7 +2298,7 @@
         <v>13.33</v>
       </c>
       <c r="J22" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="K22" s="1">
         <v>11.7</v>
@@ -2301,7 +2322,7 @@
         <v>14.23</v>
       </c>
       <c r="R22" s="1">
-        <v>10.13</v>
+        <v>10.130000000000001</v>
       </c>
       <c r="S22" s="1">
         <v>5.59</v>
@@ -2310,10 +2331,10 @@
         <v>5.41</v>
       </c>
       <c r="U22" s="1">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="V22" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="W22" s="1" t="s">
         <v>62</v>
@@ -2328,988 +2349,1063 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
-    <row r="101" ht="14.25" customHeight="1"/>
-    <row r="102" ht="14.25" customHeight="1"/>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
-    <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
-    <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
-    <row r="111" ht="14.25" customHeight="1"/>
-    <row r="112" ht="14.25" customHeight="1"/>
-    <row r="113" ht="14.25" customHeight="1"/>
-    <row r="114" ht="14.25" customHeight="1"/>
-    <row r="115" ht="14.25" customHeight="1"/>
-    <row r="116" ht="14.25" customHeight="1"/>
-    <row r="117" ht="14.25" customHeight="1"/>
-    <row r="118" ht="14.25" customHeight="1"/>
-    <row r="119" ht="14.25" customHeight="1"/>
-    <row r="120" ht="14.25" customHeight="1"/>
-    <row r="121" ht="14.25" customHeight="1"/>
-    <row r="122" ht="14.25" customHeight="1"/>
-    <row r="123" ht="14.25" customHeight="1"/>
-    <row r="124" ht="14.25" customHeight="1"/>
-    <row r="125" ht="14.25" customHeight="1"/>
-    <row r="126" ht="14.25" customHeight="1"/>
-    <row r="127" ht="14.25" customHeight="1"/>
-    <row r="128" ht="14.25" customHeight="1"/>
-    <row r="129" ht="14.25" customHeight="1"/>
-    <row r="130" ht="14.25" customHeight="1"/>
-    <row r="131" ht="14.25" customHeight="1"/>
-    <row r="132" ht="14.25" customHeight="1"/>
-    <row r="133" ht="14.25" customHeight="1"/>
-    <row r="134" ht="14.25" customHeight="1"/>
-    <row r="135" ht="14.25" customHeight="1"/>
-    <row r="136" ht="14.25" customHeight="1"/>
-    <row r="137" ht="14.25" customHeight="1"/>
-    <row r="138" ht="14.25" customHeight="1"/>
-    <row r="139" ht="14.25" customHeight="1"/>
-    <row r="140" ht="14.25" customHeight="1"/>
-    <row r="141" ht="14.25" customHeight="1"/>
-    <row r="142" ht="14.25" customHeight="1"/>
-    <row r="143" ht="14.25" customHeight="1"/>
-    <row r="144" ht="14.25" customHeight="1"/>
-    <row r="145" ht="14.25" customHeight="1"/>
-    <row r="146" ht="14.25" customHeight="1"/>
-    <row r="147" ht="14.25" customHeight="1"/>
-    <row r="148" ht="14.25" customHeight="1"/>
-    <row r="149" ht="14.25" customHeight="1"/>
-    <row r="150" ht="14.25" customHeight="1"/>
-    <row r="151" ht="14.25" customHeight="1"/>
-    <row r="152" ht="14.25" customHeight="1"/>
-    <row r="153" ht="14.25" customHeight="1"/>
-    <row r="154" ht="14.25" customHeight="1"/>
-    <row r="155" ht="14.25" customHeight="1"/>
-    <row r="156" ht="14.25" customHeight="1"/>
-    <row r="157" ht="14.25" customHeight="1"/>
-    <row r="158" ht="14.25" customHeight="1"/>
-    <row r="159" ht="14.25" customHeight="1"/>
-    <row r="160" ht="14.25" customHeight="1"/>
-    <row r="161" ht="14.25" customHeight="1"/>
-    <row r="162" ht="14.25" customHeight="1"/>
-    <row r="163" ht="14.25" customHeight="1"/>
-    <row r="164" ht="14.25" customHeight="1"/>
-    <row r="165" ht="14.25" customHeight="1"/>
-    <row r="166" ht="14.25" customHeight="1"/>
-    <row r="167" ht="14.25" customHeight="1"/>
-    <row r="168" ht="14.25" customHeight="1"/>
-    <row r="169" ht="14.25" customHeight="1"/>
-    <row r="170" ht="14.25" customHeight="1"/>
-    <row r="171" ht="14.25" customHeight="1"/>
-    <row r="172" ht="14.25" customHeight="1"/>
-    <row r="173" ht="14.25" customHeight="1"/>
-    <row r="174" ht="14.25" customHeight="1"/>
-    <row r="175" ht="14.25" customHeight="1"/>
-    <row r="176" ht="14.25" customHeight="1"/>
-    <row r="177" ht="14.25" customHeight="1"/>
-    <row r="178" ht="14.25" customHeight="1"/>
-    <row r="179" ht="14.25" customHeight="1"/>
-    <row r="180" ht="14.25" customHeight="1"/>
-    <row r="181" ht="14.25" customHeight="1"/>
-    <row r="182" ht="14.25" customHeight="1"/>
-    <row r="183" ht="14.25" customHeight="1"/>
-    <row r="184" ht="14.25" customHeight="1"/>
-    <row r="185" ht="14.25" customHeight="1"/>
-    <row r="186" ht="14.25" customHeight="1"/>
-    <row r="187" ht="14.25" customHeight="1"/>
-    <row r="188" ht="14.25" customHeight="1"/>
-    <row r="189" ht="14.25" customHeight="1"/>
-    <row r="190" ht="14.25" customHeight="1"/>
-    <row r="191" ht="14.25" customHeight="1"/>
-    <row r="192" ht="14.25" customHeight="1"/>
-    <row r="193" ht="14.25" customHeight="1"/>
-    <row r="194" ht="14.25" customHeight="1"/>
-    <row r="195" ht="14.25" customHeight="1"/>
-    <row r="196" ht="14.25" customHeight="1"/>
-    <row r="197" ht="14.25" customHeight="1"/>
-    <row r="198" ht="14.25" customHeight="1"/>
-    <row r="199" ht="14.25" customHeight="1"/>
-    <row r="200" ht="14.25" customHeight="1"/>
-    <row r="201" ht="14.25" customHeight="1"/>
-    <row r="202" ht="14.25" customHeight="1"/>
-    <row r="203" ht="14.25" customHeight="1"/>
-    <row r="204" ht="14.25" customHeight="1"/>
-    <row r="205" ht="14.25" customHeight="1"/>
-    <row r="206" ht="14.25" customHeight="1"/>
-    <row r="207" ht="14.25" customHeight="1"/>
-    <row r="208" ht="14.25" customHeight="1"/>
-    <row r="209" ht="14.25" customHeight="1"/>
-    <row r="210" ht="14.25" customHeight="1"/>
-    <row r="211" ht="14.25" customHeight="1"/>
-    <row r="212" ht="14.25" customHeight="1"/>
-    <row r="213" ht="14.25" customHeight="1"/>
-    <row r="214" ht="14.25" customHeight="1"/>
-    <row r="215" ht="14.25" customHeight="1"/>
-    <row r="216" ht="14.25" customHeight="1"/>
-    <row r="217" ht="14.25" customHeight="1"/>
-    <row r="218" ht="14.25" customHeight="1"/>
-    <row r="219" ht="14.25" customHeight="1"/>
-    <row r="220" ht="14.25" customHeight="1"/>
-    <row r="221" ht="14.25" customHeight="1"/>
-    <row r="222" ht="14.25" customHeight="1"/>
-    <row r="223" ht="14.25" customHeight="1"/>
-    <row r="224" ht="14.25" customHeight="1"/>
-    <row r="225" ht="14.25" customHeight="1"/>
-    <row r="226" ht="14.25" customHeight="1"/>
-    <row r="227" ht="14.25" customHeight="1"/>
-    <row r="228" ht="14.25" customHeight="1"/>
-    <row r="229" ht="14.25" customHeight="1"/>
-    <row r="230" ht="14.25" customHeight="1"/>
-    <row r="231" ht="14.25" customHeight="1"/>
-    <row r="232" ht="14.25" customHeight="1"/>
-    <row r="233" ht="14.25" customHeight="1"/>
-    <row r="234" ht="14.25" customHeight="1"/>
-    <row r="235" ht="14.25" customHeight="1"/>
-    <row r="236" ht="14.25" customHeight="1"/>
-    <row r="237" ht="14.25" customHeight="1"/>
-    <row r="238" ht="14.25" customHeight="1"/>
-    <row r="239" ht="14.25" customHeight="1"/>
-    <row r="240" ht="14.25" customHeight="1"/>
-    <row r="241" ht="14.25" customHeight="1"/>
-    <row r="242" ht="14.25" customHeight="1"/>
-    <row r="243" ht="14.25" customHeight="1"/>
-    <row r="244" ht="14.25" customHeight="1"/>
-    <row r="245" ht="14.25" customHeight="1"/>
-    <row r="246" ht="14.25" customHeight="1"/>
-    <row r="247" ht="14.25" customHeight="1"/>
-    <row r="248" ht="14.25" customHeight="1"/>
-    <row r="249" ht="14.25" customHeight="1"/>
-    <row r="250" ht="14.25" customHeight="1"/>
-    <row r="251" ht="14.25" customHeight="1"/>
-    <row r="252" ht="14.25" customHeight="1"/>
-    <row r="253" ht="14.25" customHeight="1"/>
-    <row r="254" ht="14.25" customHeight="1"/>
-    <row r="255" ht="14.25" customHeight="1"/>
-    <row r="256" ht="14.25" customHeight="1"/>
-    <row r="257" ht="14.25" customHeight="1"/>
-    <row r="258" ht="14.25" customHeight="1"/>
-    <row r="259" ht="14.25" customHeight="1"/>
-    <row r="260" ht="14.25" customHeight="1"/>
-    <row r="261" ht="14.25" customHeight="1"/>
-    <row r="262" ht="14.25" customHeight="1"/>
-    <row r="263" ht="14.25" customHeight="1"/>
-    <row r="264" ht="14.25" customHeight="1"/>
-    <row r="265" ht="14.25" customHeight="1"/>
-    <row r="266" ht="14.25" customHeight="1"/>
-    <row r="267" ht="14.25" customHeight="1"/>
-    <row r="268" ht="14.25" customHeight="1"/>
-    <row r="269" ht="14.25" customHeight="1"/>
-    <row r="270" ht="14.25" customHeight="1"/>
-    <row r="271" ht="14.25" customHeight="1"/>
-    <row r="272" ht="14.25" customHeight="1"/>
-    <row r="273" ht="14.25" customHeight="1"/>
-    <row r="274" ht="14.25" customHeight="1"/>
-    <row r="275" ht="14.25" customHeight="1"/>
-    <row r="276" ht="14.25" customHeight="1"/>
-    <row r="277" ht="14.25" customHeight="1"/>
-    <row r="278" ht="14.25" customHeight="1"/>
-    <row r="279" ht="14.25" customHeight="1"/>
-    <row r="280" ht="14.25" customHeight="1"/>
-    <row r="281" ht="14.25" customHeight="1"/>
-    <row r="282" ht="14.25" customHeight="1"/>
-    <row r="283" ht="14.25" customHeight="1"/>
-    <row r="284" ht="14.25" customHeight="1"/>
-    <row r="285" ht="14.25" customHeight="1"/>
-    <row r="286" ht="14.25" customHeight="1"/>
-    <row r="287" ht="14.25" customHeight="1"/>
-    <row r="288" ht="14.25" customHeight="1"/>
-    <row r="289" ht="14.25" customHeight="1"/>
-    <row r="290" ht="14.25" customHeight="1"/>
-    <row r="291" ht="14.25" customHeight="1"/>
-    <row r="292" ht="14.25" customHeight="1"/>
-    <row r="293" ht="14.25" customHeight="1"/>
-    <row r="294" ht="14.25" customHeight="1"/>
-    <row r="295" ht="14.25" customHeight="1"/>
-    <row r="296" ht="14.25" customHeight="1"/>
-    <row r="297" ht="14.25" customHeight="1"/>
-    <row r="298" ht="14.25" customHeight="1"/>
-    <row r="299" ht="14.25" customHeight="1"/>
-    <row r="300" ht="14.25" customHeight="1"/>
-    <row r="301" ht="14.25" customHeight="1"/>
-    <row r="302" ht="14.25" customHeight="1"/>
-    <row r="303" ht="14.25" customHeight="1"/>
-    <row r="304" ht="14.25" customHeight="1"/>
-    <row r="305" ht="14.25" customHeight="1"/>
-    <row r="306" ht="14.25" customHeight="1"/>
-    <row r="307" ht="14.25" customHeight="1"/>
-    <row r="308" ht="14.25" customHeight="1"/>
-    <row r="309" ht="14.25" customHeight="1"/>
-    <row r="310" ht="14.25" customHeight="1"/>
-    <row r="311" ht="14.25" customHeight="1"/>
-    <row r="312" ht="14.25" customHeight="1"/>
-    <row r="313" ht="14.25" customHeight="1"/>
-    <row r="314" ht="14.25" customHeight="1"/>
-    <row r="315" ht="14.25" customHeight="1"/>
-    <row r="316" ht="14.25" customHeight="1"/>
-    <row r="317" ht="14.25" customHeight="1"/>
-    <row r="318" ht="14.25" customHeight="1"/>
-    <row r="319" ht="14.25" customHeight="1"/>
-    <row r="320" ht="14.25" customHeight="1"/>
-    <row r="321" ht="14.25" customHeight="1"/>
-    <row r="322" ht="14.25" customHeight="1"/>
-    <row r="323" ht="14.25" customHeight="1"/>
-    <row r="324" ht="14.25" customHeight="1"/>
-    <row r="325" ht="14.25" customHeight="1"/>
-    <row r="326" ht="14.25" customHeight="1"/>
-    <row r="327" ht="14.25" customHeight="1"/>
-    <row r="328" ht="14.25" customHeight="1"/>
-    <row r="329" ht="14.25" customHeight="1"/>
-    <row r="330" ht="14.25" customHeight="1"/>
-    <row r="331" ht="14.25" customHeight="1"/>
-    <row r="332" ht="14.25" customHeight="1"/>
-    <row r="333" ht="14.25" customHeight="1"/>
-    <row r="334" ht="14.25" customHeight="1"/>
-    <row r="335" ht="14.25" customHeight="1"/>
-    <row r="336" ht="14.25" customHeight="1"/>
-    <row r="337" ht="14.25" customHeight="1"/>
-    <row r="338" ht="14.25" customHeight="1"/>
-    <row r="339" ht="14.25" customHeight="1"/>
-    <row r="340" ht="14.25" customHeight="1"/>
-    <row r="341" ht="14.25" customHeight="1"/>
-    <row r="342" ht="14.25" customHeight="1"/>
-    <row r="343" ht="14.25" customHeight="1"/>
-    <row r="344" ht="14.25" customHeight="1"/>
-    <row r="345" ht="14.25" customHeight="1"/>
-    <row r="346" ht="14.25" customHeight="1"/>
-    <row r="347" ht="14.25" customHeight="1"/>
-    <row r="348" ht="14.25" customHeight="1"/>
-    <row r="349" ht="14.25" customHeight="1"/>
-    <row r="350" ht="14.25" customHeight="1"/>
-    <row r="351" ht="14.25" customHeight="1"/>
-    <row r="352" ht="14.25" customHeight="1"/>
-    <row r="353" ht="14.25" customHeight="1"/>
-    <row r="354" ht="14.25" customHeight="1"/>
-    <row r="355" ht="14.25" customHeight="1"/>
-    <row r="356" ht="14.25" customHeight="1"/>
-    <row r="357" ht="14.25" customHeight="1"/>
-    <row r="358" ht="14.25" customHeight="1"/>
-    <row r="359" ht="14.25" customHeight="1"/>
-    <row r="360" ht="14.25" customHeight="1"/>
-    <row r="361" ht="14.25" customHeight="1"/>
-    <row r="362" ht="14.25" customHeight="1"/>
-    <row r="363" ht="14.25" customHeight="1"/>
-    <row r="364" ht="14.25" customHeight="1"/>
-    <row r="365" ht="14.25" customHeight="1"/>
-    <row r="366" ht="14.25" customHeight="1"/>
-    <row r="367" ht="14.25" customHeight="1"/>
-    <row r="368" ht="14.25" customHeight="1"/>
-    <row r="369" ht="14.25" customHeight="1"/>
-    <row r="370" ht="14.25" customHeight="1"/>
-    <row r="371" ht="14.25" customHeight="1"/>
-    <row r="372" ht="14.25" customHeight="1"/>
-    <row r="373" ht="14.25" customHeight="1"/>
-    <row r="374" ht="14.25" customHeight="1"/>
-    <row r="375" ht="14.25" customHeight="1"/>
-    <row r="376" ht="14.25" customHeight="1"/>
-    <row r="377" ht="14.25" customHeight="1"/>
-    <row r="378" ht="14.25" customHeight="1"/>
-    <row r="379" ht="14.25" customHeight="1"/>
-    <row r="380" ht="14.25" customHeight="1"/>
-    <row r="381" ht="14.25" customHeight="1"/>
-    <row r="382" ht="14.25" customHeight="1"/>
-    <row r="383" ht="14.25" customHeight="1"/>
-    <row r="384" ht="14.25" customHeight="1"/>
-    <row r="385" ht="14.25" customHeight="1"/>
-    <row r="386" ht="14.25" customHeight="1"/>
-    <row r="387" ht="14.25" customHeight="1"/>
-    <row r="388" ht="14.25" customHeight="1"/>
-    <row r="389" ht="14.25" customHeight="1"/>
-    <row r="390" ht="14.25" customHeight="1"/>
-    <row r="391" ht="14.25" customHeight="1"/>
-    <row r="392" ht="14.25" customHeight="1"/>
-    <row r="393" ht="14.25" customHeight="1"/>
-    <row r="394" ht="14.25" customHeight="1"/>
-    <row r="395" ht="14.25" customHeight="1"/>
-    <row r="396" ht="14.25" customHeight="1"/>
-    <row r="397" ht="14.25" customHeight="1"/>
-    <row r="398" ht="14.25" customHeight="1"/>
-    <row r="399" ht="14.25" customHeight="1"/>
-    <row r="400" ht="14.25" customHeight="1"/>
-    <row r="401" ht="14.25" customHeight="1"/>
-    <row r="402" ht="14.25" customHeight="1"/>
-    <row r="403" ht="14.25" customHeight="1"/>
-    <row r="404" ht="14.25" customHeight="1"/>
-    <row r="405" ht="14.25" customHeight="1"/>
-    <row r="406" ht="14.25" customHeight="1"/>
-    <row r="407" ht="14.25" customHeight="1"/>
-    <row r="408" ht="14.25" customHeight="1"/>
-    <row r="409" ht="14.25" customHeight="1"/>
-    <row r="410" ht="14.25" customHeight="1"/>
-    <row r="411" ht="14.25" customHeight="1"/>
-    <row r="412" ht="14.25" customHeight="1"/>
-    <row r="413" ht="14.25" customHeight="1"/>
-    <row r="414" ht="14.25" customHeight="1"/>
-    <row r="415" ht="14.25" customHeight="1"/>
-    <row r="416" ht="14.25" customHeight="1"/>
-    <row r="417" ht="14.25" customHeight="1"/>
-    <row r="418" ht="14.25" customHeight="1"/>
-    <row r="419" ht="14.25" customHeight="1"/>
-    <row r="420" ht="14.25" customHeight="1"/>
-    <row r="421" ht="14.25" customHeight="1"/>
-    <row r="422" ht="14.25" customHeight="1"/>
-    <row r="423" ht="14.25" customHeight="1"/>
-    <row r="424" ht="14.25" customHeight="1"/>
-    <row r="425" ht="14.25" customHeight="1"/>
-    <row r="426" ht="14.25" customHeight="1"/>
-    <row r="427" ht="14.25" customHeight="1"/>
-    <row r="428" ht="14.25" customHeight="1"/>
-    <row r="429" ht="14.25" customHeight="1"/>
-    <row r="430" ht="14.25" customHeight="1"/>
-    <row r="431" ht="14.25" customHeight="1"/>
-    <row r="432" ht="14.25" customHeight="1"/>
-    <row r="433" ht="14.25" customHeight="1"/>
-    <row r="434" ht="14.25" customHeight="1"/>
-    <row r="435" ht="14.25" customHeight="1"/>
-    <row r="436" ht="14.25" customHeight="1"/>
-    <row r="437" ht="14.25" customHeight="1"/>
-    <row r="438" ht="14.25" customHeight="1"/>
-    <row r="439" ht="14.25" customHeight="1"/>
-    <row r="440" ht="14.25" customHeight="1"/>
-    <row r="441" ht="14.25" customHeight="1"/>
-    <row r="442" ht="14.25" customHeight="1"/>
-    <row r="443" ht="14.25" customHeight="1"/>
-    <row r="444" ht="14.25" customHeight="1"/>
-    <row r="445" ht="14.25" customHeight="1"/>
-    <row r="446" ht="14.25" customHeight="1"/>
-    <row r="447" ht="14.25" customHeight="1"/>
-    <row r="448" ht="14.25" customHeight="1"/>
-    <row r="449" ht="14.25" customHeight="1"/>
-    <row r="450" ht="14.25" customHeight="1"/>
-    <row r="451" ht="14.25" customHeight="1"/>
-    <row r="452" ht="14.25" customHeight="1"/>
-    <row r="453" ht="14.25" customHeight="1"/>
-    <row r="454" ht="14.25" customHeight="1"/>
-    <row r="455" ht="14.25" customHeight="1"/>
-    <row r="456" ht="14.25" customHeight="1"/>
-    <row r="457" ht="14.25" customHeight="1"/>
-    <row r="458" ht="14.25" customHeight="1"/>
-    <row r="459" ht="14.25" customHeight="1"/>
-    <row r="460" ht="14.25" customHeight="1"/>
-    <row r="461" ht="14.25" customHeight="1"/>
-    <row r="462" ht="14.25" customHeight="1"/>
-    <row r="463" ht="14.25" customHeight="1"/>
-    <row r="464" ht="14.25" customHeight="1"/>
-    <row r="465" ht="14.25" customHeight="1"/>
-    <row r="466" ht="14.25" customHeight="1"/>
-    <row r="467" ht="14.25" customHeight="1"/>
-    <row r="468" ht="14.25" customHeight="1"/>
-    <row r="469" ht="14.25" customHeight="1"/>
-    <row r="470" ht="14.25" customHeight="1"/>
-    <row r="471" ht="14.25" customHeight="1"/>
-    <row r="472" ht="14.25" customHeight="1"/>
-    <row r="473" ht="14.25" customHeight="1"/>
-    <row r="474" ht="14.25" customHeight="1"/>
-    <row r="475" ht="14.25" customHeight="1"/>
-    <row r="476" ht="14.25" customHeight="1"/>
-    <row r="477" ht="14.25" customHeight="1"/>
-    <row r="478" ht="14.25" customHeight="1"/>
-    <row r="479" ht="14.25" customHeight="1"/>
-    <row r="480" ht="14.25" customHeight="1"/>
-    <row r="481" ht="14.25" customHeight="1"/>
-    <row r="482" ht="14.25" customHeight="1"/>
-    <row r="483" ht="14.25" customHeight="1"/>
-    <row r="484" ht="14.25" customHeight="1"/>
-    <row r="485" ht="14.25" customHeight="1"/>
-    <row r="486" ht="14.25" customHeight="1"/>
-    <row r="487" ht="14.25" customHeight="1"/>
-    <row r="488" ht="14.25" customHeight="1"/>
-    <row r="489" ht="14.25" customHeight="1"/>
-    <row r="490" ht="14.25" customHeight="1"/>
-    <row r="491" ht="14.25" customHeight="1"/>
-    <row r="492" ht="14.25" customHeight="1"/>
-    <row r="493" ht="14.25" customHeight="1"/>
-    <row r="494" ht="14.25" customHeight="1"/>
-    <row r="495" ht="14.25" customHeight="1"/>
-    <row r="496" ht="14.25" customHeight="1"/>
-    <row r="497" ht="14.25" customHeight="1"/>
-    <row r="498" ht="14.25" customHeight="1"/>
-    <row r="499" ht="14.25" customHeight="1"/>
-    <row r="500" ht="14.25" customHeight="1"/>
-    <row r="501" ht="14.25" customHeight="1"/>
-    <row r="502" ht="14.25" customHeight="1"/>
-    <row r="503" ht="14.25" customHeight="1"/>
-    <row r="504" ht="14.25" customHeight="1"/>
-    <row r="505" ht="14.25" customHeight="1"/>
-    <row r="506" ht="14.25" customHeight="1"/>
-    <row r="507" ht="14.25" customHeight="1"/>
-    <row r="508" ht="14.25" customHeight="1"/>
-    <row r="509" ht="14.25" customHeight="1"/>
-    <row r="510" ht="14.25" customHeight="1"/>
-    <row r="511" ht="14.25" customHeight="1"/>
-    <row r="512" ht="14.25" customHeight="1"/>
-    <row r="513" ht="14.25" customHeight="1"/>
-    <row r="514" ht="14.25" customHeight="1"/>
-    <row r="515" ht="14.25" customHeight="1"/>
-    <row r="516" ht="14.25" customHeight="1"/>
-    <row r="517" ht="14.25" customHeight="1"/>
-    <row r="518" ht="14.25" customHeight="1"/>
-    <row r="519" ht="14.25" customHeight="1"/>
-    <row r="520" ht="14.25" customHeight="1"/>
-    <row r="521" ht="14.25" customHeight="1"/>
-    <row r="522" ht="14.25" customHeight="1"/>
-    <row r="523" ht="14.25" customHeight="1"/>
-    <row r="524" ht="14.25" customHeight="1"/>
-    <row r="525" ht="14.25" customHeight="1"/>
-    <row r="526" ht="14.25" customHeight="1"/>
-    <row r="527" ht="14.25" customHeight="1"/>
-    <row r="528" ht="14.25" customHeight="1"/>
-    <row r="529" ht="14.25" customHeight="1"/>
-    <row r="530" ht="14.25" customHeight="1"/>
-    <row r="531" ht="14.25" customHeight="1"/>
-    <row r="532" ht="14.25" customHeight="1"/>
-    <row r="533" ht="14.25" customHeight="1"/>
-    <row r="534" ht="14.25" customHeight="1"/>
-    <row r="535" ht="14.25" customHeight="1"/>
-    <row r="536" ht="14.25" customHeight="1"/>
-    <row r="537" ht="14.25" customHeight="1"/>
-    <row r="538" ht="14.25" customHeight="1"/>
-    <row r="539" ht="14.25" customHeight="1"/>
-    <row r="540" ht="14.25" customHeight="1"/>
-    <row r="541" ht="14.25" customHeight="1"/>
-    <row r="542" ht="14.25" customHeight="1"/>
-    <row r="543" ht="14.25" customHeight="1"/>
-    <row r="544" ht="14.25" customHeight="1"/>
-    <row r="545" ht="14.25" customHeight="1"/>
-    <row r="546" ht="14.25" customHeight="1"/>
-    <row r="547" ht="14.25" customHeight="1"/>
-    <row r="548" ht="14.25" customHeight="1"/>
-    <row r="549" ht="14.25" customHeight="1"/>
-    <row r="550" ht="14.25" customHeight="1"/>
-    <row r="551" ht="14.25" customHeight="1"/>
-    <row r="552" ht="14.25" customHeight="1"/>
-    <row r="553" ht="14.25" customHeight="1"/>
-    <row r="554" ht="14.25" customHeight="1"/>
-    <row r="555" ht="14.25" customHeight="1"/>
-    <row r="556" ht="14.25" customHeight="1"/>
-    <row r="557" ht="14.25" customHeight="1"/>
-    <row r="558" ht="14.25" customHeight="1"/>
-    <row r="559" ht="14.25" customHeight="1"/>
-    <row r="560" ht="14.25" customHeight="1"/>
-    <row r="561" ht="14.25" customHeight="1"/>
-    <row r="562" ht="14.25" customHeight="1"/>
-    <row r="563" ht="14.25" customHeight="1"/>
-    <row r="564" ht="14.25" customHeight="1"/>
-    <row r="565" ht="14.25" customHeight="1"/>
-    <row r="566" ht="14.25" customHeight="1"/>
-    <row r="567" ht="14.25" customHeight="1"/>
-    <row r="568" ht="14.25" customHeight="1"/>
-    <row r="569" ht="14.25" customHeight="1"/>
-    <row r="570" ht="14.25" customHeight="1"/>
-    <row r="571" ht="14.25" customHeight="1"/>
-    <row r="572" ht="14.25" customHeight="1"/>
-    <row r="573" ht="14.25" customHeight="1"/>
-    <row r="574" ht="14.25" customHeight="1"/>
-    <row r="575" ht="14.25" customHeight="1"/>
-    <row r="576" ht="14.25" customHeight="1"/>
-    <row r="577" ht="14.25" customHeight="1"/>
-    <row r="578" ht="14.25" customHeight="1"/>
-    <row r="579" ht="14.25" customHeight="1"/>
-    <row r="580" ht="14.25" customHeight="1"/>
-    <row r="581" ht="14.25" customHeight="1"/>
-    <row r="582" ht="14.25" customHeight="1"/>
-    <row r="583" ht="14.25" customHeight="1"/>
-    <row r="584" ht="14.25" customHeight="1"/>
-    <row r="585" ht="14.25" customHeight="1"/>
-    <row r="586" ht="14.25" customHeight="1"/>
-    <row r="587" ht="14.25" customHeight="1"/>
-    <row r="588" ht="14.25" customHeight="1"/>
-    <row r="589" ht="14.25" customHeight="1"/>
-    <row r="590" ht="14.25" customHeight="1"/>
-    <row r="591" ht="14.25" customHeight="1"/>
-    <row r="592" ht="14.25" customHeight="1"/>
-    <row r="593" ht="14.25" customHeight="1"/>
-    <row r="594" ht="14.25" customHeight="1"/>
-    <row r="595" ht="14.25" customHeight="1"/>
-    <row r="596" ht="14.25" customHeight="1"/>
-    <row r="597" ht="14.25" customHeight="1"/>
-    <row r="598" ht="14.25" customHeight="1"/>
-    <row r="599" ht="14.25" customHeight="1"/>
-    <row r="600" ht="14.25" customHeight="1"/>
-    <row r="601" ht="14.25" customHeight="1"/>
-    <row r="602" ht="14.25" customHeight="1"/>
-    <row r="603" ht="14.25" customHeight="1"/>
-    <row r="604" ht="14.25" customHeight="1"/>
-    <row r="605" ht="14.25" customHeight="1"/>
-    <row r="606" ht="14.25" customHeight="1"/>
-    <row r="607" ht="14.25" customHeight="1"/>
-    <row r="608" ht="14.25" customHeight="1"/>
-    <row r="609" ht="14.25" customHeight="1"/>
-    <row r="610" ht="14.25" customHeight="1"/>
-    <row r="611" ht="14.25" customHeight="1"/>
-    <row r="612" ht="14.25" customHeight="1"/>
-    <row r="613" ht="14.25" customHeight="1"/>
-    <row r="614" ht="14.25" customHeight="1"/>
-    <row r="615" ht="14.25" customHeight="1"/>
-    <row r="616" ht="14.25" customHeight="1"/>
-    <row r="617" ht="14.25" customHeight="1"/>
-    <row r="618" ht="14.25" customHeight="1"/>
-    <row r="619" ht="14.25" customHeight="1"/>
-    <row r="620" ht="14.25" customHeight="1"/>
-    <row r="621" ht="14.25" customHeight="1"/>
-    <row r="622" ht="14.25" customHeight="1"/>
-    <row r="623" ht="14.25" customHeight="1"/>
-    <row r="624" ht="14.25" customHeight="1"/>
-    <row r="625" ht="14.25" customHeight="1"/>
-    <row r="626" ht="14.25" customHeight="1"/>
-    <row r="627" ht="14.25" customHeight="1"/>
-    <row r="628" ht="14.25" customHeight="1"/>
-    <row r="629" ht="14.25" customHeight="1"/>
-    <row r="630" ht="14.25" customHeight="1"/>
-    <row r="631" ht="14.25" customHeight="1"/>
-    <row r="632" ht="14.25" customHeight="1"/>
-    <row r="633" ht="14.25" customHeight="1"/>
-    <row r="634" ht="14.25" customHeight="1"/>
-    <row r="635" ht="14.25" customHeight="1"/>
-    <row r="636" ht="14.25" customHeight="1"/>
-    <row r="637" ht="14.25" customHeight="1"/>
-    <row r="638" ht="14.25" customHeight="1"/>
-    <row r="639" ht="14.25" customHeight="1"/>
-    <row r="640" ht="14.25" customHeight="1"/>
-    <row r="641" ht="14.25" customHeight="1"/>
-    <row r="642" ht="14.25" customHeight="1"/>
-    <row r="643" ht="14.25" customHeight="1"/>
-    <row r="644" ht="14.25" customHeight="1"/>
-    <row r="645" ht="14.25" customHeight="1"/>
-    <row r="646" ht="14.25" customHeight="1"/>
-    <row r="647" ht="14.25" customHeight="1"/>
-    <row r="648" ht="14.25" customHeight="1"/>
-    <row r="649" ht="14.25" customHeight="1"/>
-    <row r="650" ht="14.25" customHeight="1"/>
-    <row r="651" ht="14.25" customHeight="1"/>
-    <row r="652" ht="14.25" customHeight="1"/>
-    <row r="653" ht="14.25" customHeight="1"/>
-    <row r="654" ht="14.25" customHeight="1"/>
-    <row r="655" ht="14.25" customHeight="1"/>
-    <row r="656" ht="14.25" customHeight="1"/>
-    <row r="657" ht="14.25" customHeight="1"/>
-    <row r="658" ht="14.25" customHeight="1"/>
-    <row r="659" ht="14.25" customHeight="1"/>
-    <row r="660" ht="14.25" customHeight="1"/>
-    <row r="661" ht="14.25" customHeight="1"/>
-    <row r="662" ht="14.25" customHeight="1"/>
-    <row r="663" ht="14.25" customHeight="1"/>
-    <row r="664" ht="14.25" customHeight="1"/>
-    <row r="665" ht="14.25" customHeight="1"/>
-    <row r="666" ht="14.25" customHeight="1"/>
-    <row r="667" ht="14.25" customHeight="1"/>
-    <row r="668" ht="14.25" customHeight="1"/>
-    <row r="669" ht="14.25" customHeight="1"/>
-    <row r="670" ht="14.25" customHeight="1"/>
-    <row r="671" ht="14.25" customHeight="1"/>
-    <row r="672" ht="14.25" customHeight="1"/>
-    <row r="673" ht="14.25" customHeight="1"/>
-    <row r="674" ht="14.25" customHeight="1"/>
-    <row r="675" ht="14.25" customHeight="1"/>
-    <row r="676" ht="14.25" customHeight="1"/>
-    <row r="677" ht="14.25" customHeight="1"/>
-    <row r="678" ht="14.25" customHeight="1"/>
-    <row r="679" ht="14.25" customHeight="1"/>
-    <row r="680" ht="14.25" customHeight="1"/>
-    <row r="681" ht="14.25" customHeight="1"/>
-    <row r="682" ht="14.25" customHeight="1"/>
-    <row r="683" ht="14.25" customHeight="1"/>
-    <row r="684" ht="14.25" customHeight="1"/>
-    <row r="685" ht="14.25" customHeight="1"/>
-    <row r="686" ht="14.25" customHeight="1"/>
-    <row r="687" ht="14.25" customHeight="1"/>
-    <row r="688" ht="14.25" customHeight="1"/>
-    <row r="689" ht="14.25" customHeight="1"/>
-    <row r="690" ht="14.25" customHeight="1"/>
-    <row r="691" ht="14.25" customHeight="1"/>
-    <row r="692" ht="14.25" customHeight="1"/>
-    <row r="693" ht="14.25" customHeight="1"/>
-    <row r="694" ht="14.25" customHeight="1"/>
-    <row r="695" ht="14.25" customHeight="1"/>
-    <row r="696" ht="14.25" customHeight="1"/>
-    <row r="697" ht="14.25" customHeight="1"/>
-    <row r="698" ht="14.25" customHeight="1"/>
-    <row r="699" ht="14.25" customHeight="1"/>
-    <row r="700" ht="14.25" customHeight="1"/>
-    <row r="701" ht="14.25" customHeight="1"/>
-    <row r="702" ht="14.25" customHeight="1"/>
-    <row r="703" ht="14.25" customHeight="1"/>
-    <row r="704" ht="14.25" customHeight="1"/>
-    <row r="705" ht="14.25" customHeight="1"/>
-    <row r="706" ht="14.25" customHeight="1"/>
-    <row r="707" ht="14.25" customHeight="1"/>
-    <row r="708" ht="14.25" customHeight="1"/>
-    <row r="709" ht="14.25" customHeight="1"/>
-    <row r="710" ht="14.25" customHeight="1"/>
-    <row r="711" ht="14.25" customHeight="1"/>
-    <row r="712" ht="14.25" customHeight="1"/>
-    <row r="713" ht="14.25" customHeight="1"/>
-    <row r="714" ht="14.25" customHeight="1"/>
-    <row r="715" ht="14.25" customHeight="1"/>
-    <row r="716" ht="14.25" customHeight="1"/>
-    <row r="717" ht="14.25" customHeight="1"/>
-    <row r="718" ht="14.25" customHeight="1"/>
-    <row r="719" ht="14.25" customHeight="1"/>
-    <row r="720" ht="14.25" customHeight="1"/>
-    <row r="721" ht="14.25" customHeight="1"/>
-    <row r="722" ht="14.25" customHeight="1"/>
-    <row r="723" ht="14.25" customHeight="1"/>
-    <row r="724" ht="14.25" customHeight="1"/>
-    <row r="725" ht="14.25" customHeight="1"/>
-    <row r="726" ht="14.25" customHeight="1"/>
-    <row r="727" ht="14.25" customHeight="1"/>
-    <row r="728" ht="14.25" customHeight="1"/>
-    <row r="729" ht="14.25" customHeight="1"/>
-    <row r="730" ht="14.25" customHeight="1"/>
-    <row r="731" ht="14.25" customHeight="1"/>
-    <row r="732" ht="14.25" customHeight="1"/>
-    <row r="733" ht="14.25" customHeight="1"/>
-    <row r="734" ht="14.25" customHeight="1"/>
-    <row r="735" ht="14.25" customHeight="1"/>
-    <row r="736" ht="14.25" customHeight="1"/>
-    <row r="737" ht="14.25" customHeight="1"/>
-    <row r="738" ht="14.25" customHeight="1"/>
-    <row r="739" ht="14.25" customHeight="1"/>
-    <row r="740" ht="14.25" customHeight="1"/>
-    <row r="741" ht="14.25" customHeight="1"/>
-    <row r="742" ht="14.25" customHeight="1"/>
-    <row r="743" ht="14.25" customHeight="1"/>
-    <row r="744" ht="14.25" customHeight="1"/>
-    <row r="745" ht="14.25" customHeight="1"/>
-    <row r="746" ht="14.25" customHeight="1"/>
-    <row r="747" ht="14.25" customHeight="1"/>
-    <row r="748" ht="14.25" customHeight="1"/>
-    <row r="749" ht="14.25" customHeight="1"/>
-    <row r="750" ht="14.25" customHeight="1"/>
-    <row r="751" ht="14.25" customHeight="1"/>
-    <row r="752" ht="14.25" customHeight="1"/>
-    <row r="753" ht="14.25" customHeight="1"/>
-    <row r="754" ht="14.25" customHeight="1"/>
-    <row r="755" ht="14.25" customHeight="1"/>
-    <row r="756" ht="14.25" customHeight="1"/>
-    <row r="757" ht="14.25" customHeight="1"/>
-    <row r="758" ht="14.25" customHeight="1"/>
-    <row r="759" ht="14.25" customHeight="1"/>
-    <row r="760" ht="14.25" customHeight="1"/>
-    <row r="761" ht="14.25" customHeight="1"/>
-    <row r="762" ht="14.25" customHeight="1"/>
-    <row r="763" ht="14.25" customHeight="1"/>
-    <row r="764" ht="14.25" customHeight="1"/>
-    <row r="765" ht="14.25" customHeight="1"/>
-    <row r="766" ht="14.25" customHeight="1"/>
-    <row r="767" ht="14.25" customHeight="1"/>
-    <row r="768" ht="14.25" customHeight="1"/>
-    <row r="769" ht="14.25" customHeight="1"/>
-    <row r="770" ht="14.25" customHeight="1"/>
-    <row r="771" ht="14.25" customHeight="1"/>
-    <row r="772" ht="14.25" customHeight="1"/>
-    <row r="773" ht="14.25" customHeight="1"/>
-    <row r="774" ht="14.25" customHeight="1"/>
-    <row r="775" ht="14.25" customHeight="1"/>
-    <row r="776" ht="14.25" customHeight="1"/>
-    <row r="777" ht="14.25" customHeight="1"/>
-    <row r="778" ht="14.25" customHeight="1"/>
-    <row r="779" ht="14.25" customHeight="1"/>
-    <row r="780" ht="14.25" customHeight="1"/>
-    <row r="781" ht="14.25" customHeight="1"/>
-    <row r="782" ht="14.25" customHeight="1"/>
-    <row r="783" ht="14.25" customHeight="1"/>
-    <row r="784" ht="14.25" customHeight="1"/>
-    <row r="785" ht="14.25" customHeight="1"/>
-    <row r="786" ht="14.25" customHeight="1"/>
-    <row r="787" ht="14.25" customHeight="1"/>
-    <row r="788" ht="14.25" customHeight="1"/>
-    <row r="789" ht="14.25" customHeight="1"/>
-    <row r="790" ht="14.25" customHeight="1"/>
-    <row r="791" ht="14.25" customHeight="1"/>
-    <row r="792" ht="14.25" customHeight="1"/>
-    <row r="793" ht="14.25" customHeight="1"/>
-    <row r="794" ht="14.25" customHeight="1"/>
-    <row r="795" ht="14.25" customHeight="1"/>
-    <row r="796" ht="14.25" customHeight="1"/>
-    <row r="797" ht="14.25" customHeight="1"/>
-    <row r="798" ht="14.25" customHeight="1"/>
-    <row r="799" ht="14.25" customHeight="1"/>
-    <row r="800" ht="14.25" customHeight="1"/>
-    <row r="801" ht="14.25" customHeight="1"/>
-    <row r="802" ht="14.25" customHeight="1"/>
-    <row r="803" ht="14.25" customHeight="1"/>
-    <row r="804" ht="14.25" customHeight="1"/>
-    <row r="805" ht="14.25" customHeight="1"/>
-    <row r="806" ht="14.25" customHeight="1"/>
-    <row r="807" ht="14.25" customHeight="1"/>
-    <row r="808" ht="14.25" customHeight="1"/>
-    <row r="809" ht="14.25" customHeight="1"/>
-    <row r="810" ht="14.25" customHeight="1"/>
-    <row r="811" ht="14.25" customHeight="1"/>
-    <row r="812" ht="14.25" customHeight="1"/>
-    <row r="813" ht="14.25" customHeight="1"/>
-    <row r="814" ht="14.25" customHeight="1"/>
-    <row r="815" ht="14.25" customHeight="1"/>
-    <row r="816" ht="14.25" customHeight="1"/>
-    <row r="817" ht="14.25" customHeight="1"/>
-    <row r="818" ht="14.25" customHeight="1"/>
-    <row r="819" ht="14.25" customHeight="1"/>
-    <row r="820" ht="14.25" customHeight="1"/>
-    <row r="821" ht="14.25" customHeight="1"/>
-    <row r="822" ht="14.25" customHeight="1"/>
-    <row r="823" ht="14.25" customHeight="1"/>
-    <row r="824" ht="14.25" customHeight="1"/>
-    <row r="825" ht="14.25" customHeight="1"/>
-    <row r="826" ht="14.25" customHeight="1"/>
-    <row r="827" ht="14.25" customHeight="1"/>
-    <row r="828" ht="14.25" customHeight="1"/>
-    <row r="829" ht="14.25" customHeight="1"/>
-    <row r="830" ht="14.25" customHeight="1"/>
-    <row r="831" ht="14.25" customHeight="1"/>
-    <row r="832" ht="14.25" customHeight="1"/>
-    <row r="833" ht="14.25" customHeight="1"/>
-    <row r="834" ht="14.25" customHeight="1"/>
-    <row r="835" ht="14.25" customHeight="1"/>
-    <row r="836" ht="14.25" customHeight="1"/>
-    <row r="837" ht="14.25" customHeight="1"/>
-    <row r="838" ht="14.25" customHeight="1"/>
-    <row r="839" ht="14.25" customHeight="1"/>
-    <row r="840" ht="14.25" customHeight="1"/>
-    <row r="841" ht="14.25" customHeight="1"/>
-    <row r="842" ht="14.25" customHeight="1"/>
-    <row r="843" ht="14.25" customHeight="1"/>
-    <row r="844" ht="14.25" customHeight="1"/>
-    <row r="845" ht="14.25" customHeight="1"/>
-    <row r="846" ht="14.25" customHeight="1"/>
-    <row r="847" ht="14.25" customHeight="1"/>
-    <row r="848" ht="14.25" customHeight="1"/>
-    <row r="849" ht="14.25" customHeight="1"/>
-    <row r="850" ht="14.25" customHeight="1"/>
-    <row r="851" ht="14.25" customHeight="1"/>
-    <row r="852" ht="14.25" customHeight="1"/>
-    <row r="853" ht="14.25" customHeight="1"/>
-    <row r="854" ht="14.25" customHeight="1"/>
-    <row r="855" ht="14.25" customHeight="1"/>
-    <row r="856" ht="14.25" customHeight="1"/>
-    <row r="857" ht="14.25" customHeight="1"/>
-    <row r="858" ht="14.25" customHeight="1"/>
-    <row r="859" ht="14.25" customHeight="1"/>
-    <row r="860" ht="14.25" customHeight="1"/>
-    <row r="861" ht="14.25" customHeight="1"/>
-    <row r="862" ht="14.25" customHeight="1"/>
-    <row r="863" ht="14.25" customHeight="1"/>
-    <row r="864" ht="14.25" customHeight="1"/>
-    <row r="865" ht="14.25" customHeight="1"/>
-    <row r="866" ht="14.25" customHeight="1"/>
-    <row r="867" ht="14.25" customHeight="1"/>
-    <row r="868" ht="14.25" customHeight="1"/>
-    <row r="869" ht="14.25" customHeight="1"/>
-    <row r="870" ht="14.25" customHeight="1"/>
-    <row r="871" ht="14.25" customHeight="1"/>
-    <row r="872" ht="14.25" customHeight="1"/>
-    <row r="873" ht="14.25" customHeight="1"/>
-    <row r="874" ht="14.25" customHeight="1"/>
-    <row r="875" ht="14.25" customHeight="1"/>
-    <row r="876" ht="14.25" customHeight="1"/>
-    <row r="877" ht="14.25" customHeight="1"/>
-    <row r="878" ht="14.25" customHeight="1"/>
-    <row r="879" ht="14.25" customHeight="1"/>
-    <row r="880" ht="14.25" customHeight="1"/>
-    <row r="881" ht="14.25" customHeight="1"/>
-    <row r="882" ht="14.25" customHeight="1"/>
-    <row r="883" ht="14.25" customHeight="1"/>
-    <row r="884" ht="14.25" customHeight="1"/>
-    <row r="885" ht="14.25" customHeight="1"/>
-    <row r="886" ht="14.25" customHeight="1"/>
-    <row r="887" ht="14.25" customHeight="1"/>
-    <row r="888" ht="14.25" customHeight="1"/>
-    <row r="889" ht="14.25" customHeight="1"/>
-    <row r="890" ht="14.25" customHeight="1"/>
-    <row r="891" ht="14.25" customHeight="1"/>
-    <row r="892" ht="14.25" customHeight="1"/>
-    <row r="893" ht="14.25" customHeight="1"/>
-    <row r="894" ht="14.25" customHeight="1"/>
-    <row r="895" ht="14.25" customHeight="1"/>
-    <row r="896" ht="14.25" customHeight="1"/>
-    <row r="897" ht="14.25" customHeight="1"/>
-    <row r="898" ht="14.25" customHeight="1"/>
-    <row r="899" ht="14.25" customHeight="1"/>
-    <row r="900" ht="14.25" customHeight="1"/>
-    <row r="901" ht="14.25" customHeight="1"/>
-    <row r="902" ht="14.25" customHeight="1"/>
-    <row r="903" ht="14.25" customHeight="1"/>
-    <row r="904" ht="14.25" customHeight="1"/>
-    <row r="905" ht="14.25" customHeight="1"/>
-    <row r="906" ht="14.25" customHeight="1"/>
-    <row r="907" ht="14.25" customHeight="1"/>
-    <row r="908" ht="14.25" customHeight="1"/>
-    <row r="909" ht="14.25" customHeight="1"/>
-    <row r="910" ht="14.25" customHeight="1"/>
-    <row r="911" ht="14.25" customHeight="1"/>
-    <row r="912" ht="14.25" customHeight="1"/>
-    <row r="913" ht="14.25" customHeight="1"/>
-    <row r="914" ht="14.25" customHeight="1"/>
-    <row r="915" ht="14.25" customHeight="1"/>
-    <row r="916" ht="14.25" customHeight="1"/>
-    <row r="917" ht="14.25" customHeight="1"/>
-    <row r="918" ht="14.25" customHeight="1"/>
-    <row r="919" ht="14.25" customHeight="1"/>
-    <row r="920" ht="14.25" customHeight="1"/>
-    <row r="921" ht="14.25" customHeight="1"/>
-    <row r="922" ht="14.25" customHeight="1"/>
-    <row r="923" ht="14.25" customHeight="1"/>
-    <row r="924" ht="14.25" customHeight="1"/>
-    <row r="925" ht="14.25" customHeight="1"/>
-    <row r="926" ht="14.25" customHeight="1"/>
-    <row r="927" ht="14.25" customHeight="1"/>
-    <row r="928" ht="14.25" customHeight="1"/>
-    <row r="929" ht="14.25" customHeight="1"/>
-    <row r="930" ht="14.25" customHeight="1"/>
-    <row r="931" ht="14.25" customHeight="1"/>
-    <row r="932" ht="14.25" customHeight="1"/>
-    <row r="933" ht="14.25" customHeight="1"/>
-    <row r="934" ht="14.25" customHeight="1"/>
-    <row r="935" ht="14.25" customHeight="1"/>
-    <row r="936" ht="14.25" customHeight="1"/>
-    <row r="937" ht="14.25" customHeight="1"/>
-    <row r="938" ht="14.25" customHeight="1"/>
-    <row r="939" ht="14.25" customHeight="1"/>
-    <row r="940" ht="14.25" customHeight="1"/>
-    <row r="941" ht="14.25" customHeight="1"/>
-    <row r="942" ht="14.25" customHeight="1"/>
-    <row r="943" ht="14.25" customHeight="1"/>
-    <row r="944" ht="14.25" customHeight="1"/>
-    <row r="945" ht="14.25" customHeight="1"/>
-    <row r="946" ht="14.25" customHeight="1"/>
-    <row r="947" ht="14.25" customHeight="1"/>
-    <row r="948" ht="14.25" customHeight="1"/>
-    <row r="949" ht="14.25" customHeight="1"/>
-    <row r="950" ht="14.25" customHeight="1"/>
-    <row r="951" ht="14.25" customHeight="1"/>
-    <row r="952" ht="14.25" customHeight="1"/>
-    <row r="953" ht="14.25" customHeight="1"/>
-    <row r="954" ht="14.25" customHeight="1"/>
-    <row r="955" ht="14.25" customHeight="1"/>
-    <row r="956" ht="14.25" customHeight="1"/>
-    <row r="957" ht="14.25" customHeight="1"/>
-    <row r="958" ht="14.25" customHeight="1"/>
-    <row r="959" ht="14.25" customHeight="1"/>
-    <row r="960" ht="14.25" customHeight="1"/>
-    <row r="961" ht="14.25" customHeight="1"/>
-    <row r="962" ht="14.25" customHeight="1"/>
-    <row r="963" ht="14.25" customHeight="1"/>
-    <row r="964" ht="14.25" customHeight="1"/>
-    <row r="965" ht="14.25" customHeight="1"/>
-    <row r="966" ht="14.25" customHeight="1"/>
-    <row r="967" ht="14.25" customHeight="1"/>
-    <row r="968" ht="14.25" customHeight="1"/>
-    <row r="969" ht="14.25" customHeight="1"/>
-    <row r="970" ht="14.25" customHeight="1"/>
-    <row r="971" ht="14.25" customHeight="1"/>
-    <row r="972" ht="14.25" customHeight="1"/>
-    <row r="973" ht="14.25" customHeight="1"/>
-    <row r="974" ht="14.25" customHeight="1"/>
-    <row r="975" ht="14.25" customHeight="1"/>
-    <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1234</v>
+      </c>
+      <c r="E23" s="1">
+        <v>8</v>
+      </c>
+      <c r="F23" s="1">
+        <v>12</v>
+      </c>
+      <c r="G23" s="1">
+        <v>126.55</v>
+      </c>
+      <c r="H23" s="1">
+        <v>85.25</v>
+      </c>
+      <c r="I23" s="1">
+        <v>14.36</v>
+      </c>
+      <c r="J23" s="1">
+        <v>7</v>
+      </c>
+      <c r="K23" s="1">
+        <v>9.36</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N23" s="1">
+        <v>7.81</v>
+      </c>
+      <c r="O23" s="1">
+        <v>6.54</v>
+      </c>
+      <c r="P23" s="1">
+        <v>6.54</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>10.69</v>
+      </c>
+      <c r="R23" s="1">
+        <v>8.14</v>
+      </c>
+      <c r="S23" s="1">
+        <v>10.65</v>
+      </c>
+      <c r="T23" s="1">
+        <v>7.39</v>
+      </c>
+      <c r="U23" s="1">
+        <v>150</v>
+      </c>
+      <c r="V23" s="1">
+        <v>5</v>
+      </c>
+      <c r="W23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="X23" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z23" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>